<commit_message>
added more ri scope filter tests with expected folder and updated doc
</commit_message>
<xml_diff>
--- a/validation/reinsurance_test_case_list.xlsx
+++ b/validation/reinsurance_test_case_list.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_branch\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\joh\dev\OasisLMF_ri_scope\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FC181F-E676-4647-81EF-2D023E588705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25008196-2B24-4669-A4C5-5D59061144B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
   </bookViews>
   <sheets>
     <sheet name="reinsurance1" sheetId="1" r:id="rId1"/>
     <sheet name="reinsurance2" sheetId="2" r:id="rId2"/>
+    <sheet name="reinsurance3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">reinsurance1!$A$1:$M$64</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="205">
   <si>
     <t>FolderName</t>
   </si>
@@ -304,6 +305,354 @@
   </si>
   <si>
     <t>single contract tests</t>
+  </si>
+  <si>
+    <t>reinsurance 3 ri scope filter test list</t>
+  </si>
+  <si>
+    <t>PlacedPercent</t>
+  </si>
+  <si>
+    <t>ReinsName</t>
+  </si>
+  <si>
+    <t>PortNumber</t>
+  </si>
+  <si>
+    <t>AccNumber</t>
+  </si>
+  <si>
+    <t>LocGroup</t>
+  </si>
+  <si>
+    <t>LocNumber</t>
+  </si>
+  <si>
+    <t>CedantName</t>
+  </si>
+  <si>
+    <t>ProducerName</t>
+  </si>
+  <si>
+    <t>LOB</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>ReinsTag</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Cedant1</t>
+  </si>
+  <si>
+    <t>50% of Loc1 ceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These filter tests are designed to </t>
+  </si>
+  <si>
+    <t>Producer2</t>
+  </si>
+  <si>
+    <t>50% of Loc2 ceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">result in each unique location being ceded 50% in total, </t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>50% of Loc3 ceded</t>
+  </si>
+  <si>
+    <t>across all reinsurance contracts</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>50% of Loc4 ceded</t>
+  </si>
+  <si>
+    <t>resulting in all net losses by location being 50% of the gross loss.</t>
+  </si>
+  <si>
+    <t>ReinsTag5</t>
+  </si>
+  <si>
+    <t>50% of Loc5 ceded</t>
+  </si>
+  <si>
+    <t>LocGroup6</t>
+  </si>
+  <si>
+    <t>50% of Loc6 ceded</t>
+  </si>
+  <si>
+    <t>ReinsNumber 1-15 are the tests for the filter fields;</t>
+  </si>
+  <si>
+    <t>Cedant7 and COM</t>
+  </si>
+  <si>
+    <t>Cedant7</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>50% of Loc7 ceded</t>
+  </si>
+  <si>
+    <t>CedantName, ProducerName, LOB, LocGroup, ReinsTag</t>
+  </si>
+  <si>
+    <t>IND and IE</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>50% of Loc8 ceded</t>
+  </si>
+  <si>
+    <t>COM and ReinsTag9</t>
+  </si>
+  <si>
+    <t>ReinsTag9</t>
+  </si>
+  <si>
+    <t>50% of Loc9 ceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReinsNumber 101-115 are the equivalent tests to ReinsNumber 1-15 </t>
+  </si>
+  <si>
+    <t>All Loc 10 filters</t>
+  </si>
+  <si>
+    <t>LocGroup10</t>
+  </si>
+  <si>
+    <t>Cedant10</t>
+  </si>
+  <si>
+    <t>Producer10</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>ReinsTag10</t>
+  </si>
+  <si>
+    <t>50% of Loc10 ceded</t>
+  </si>
+  <si>
+    <t>Cedant11 or Producer12</t>
+  </si>
+  <si>
+    <t>Cedant11</t>
+  </si>
+  <si>
+    <t>50% of Loc11 ceded</t>
+  </si>
+  <si>
+    <t>Producer12</t>
+  </si>
+  <si>
+    <t>50% of Loc12 ceded</t>
+  </si>
+  <si>
+    <t>AGR or AT</t>
+  </si>
+  <si>
+    <t>AGR</t>
+  </si>
+  <si>
+    <t>50% of Loc13 ceded</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>50% of Loc14 ceded</t>
+  </si>
+  <si>
+    <t>LocGroup15 or ReinsTag16</t>
+  </si>
+  <si>
+    <t>LocGroup15</t>
+  </si>
+  <si>
+    <t>50% of Loc15 ceded</t>
+  </si>
+  <si>
+    <t>ReinsTag16</t>
+  </si>
+  <si>
+    <t>50% of Loc16 ceded</t>
+  </si>
+  <si>
+    <t>Cedant17 and IT or IT and ReinsTag18</t>
+  </si>
+  <si>
+    <t>Cedant17</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>50% of Loc17 ceded</t>
+  </si>
+  <si>
+    <t>ReinsTag18</t>
+  </si>
+  <si>
+    <t>50% of Loc18 ceded</t>
+  </si>
+  <si>
+    <t>Port4 Loc19 or CH</t>
+  </si>
+  <si>
+    <t>A11129</t>
+  </si>
+  <si>
+    <t>50% of Loc19 ceded</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>50% of Loc20 ceded</t>
+  </si>
+  <si>
+    <t>ReinsNumber1_ctrl</t>
+  </si>
+  <si>
+    <t>A11111</t>
+  </si>
+  <si>
+    <t>ReinsNumber2_ctrl</t>
+  </si>
+  <si>
+    <t>A11112</t>
+  </si>
+  <si>
+    <t>ReinsNumber3_ctrl</t>
+  </si>
+  <si>
+    <t>A11113</t>
+  </si>
+  <si>
+    <t>ReinsNumber4_ctrl</t>
+  </si>
+  <si>
+    <t>A11114</t>
+  </si>
+  <si>
+    <t>ReinsNumber5_ctrl</t>
+  </si>
+  <si>
+    <t>A11115</t>
+  </si>
+  <si>
+    <t>ReinsNumber6_ctrl</t>
+  </si>
+  <si>
+    <t>A11116</t>
+  </si>
+  <si>
+    <t>ReinsNumber7_ctrl</t>
+  </si>
+  <si>
+    <t>A11117</t>
+  </si>
+  <si>
+    <t>ReinsNumber8_ctrl</t>
+  </si>
+  <si>
+    <t>A11118</t>
+  </si>
+  <si>
+    <t>ReinsNumber9_ctrl</t>
+  </si>
+  <si>
+    <t>A11119</t>
+  </si>
+  <si>
+    <t>ReinsNumber10_ctrl</t>
+  </si>
+  <si>
+    <t>A11120</t>
+  </si>
+  <si>
+    <t>ReinsNumber11_ctrl</t>
+  </si>
+  <si>
+    <t>A11121</t>
+  </si>
+  <si>
+    <t>A11122</t>
+  </si>
+  <si>
+    <t>ReinsNumber12_ctrl</t>
+  </si>
+  <si>
+    <t>A11123</t>
+  </si>
+  <si>
+    <t>A11124</t>
+  </si>
+  <si>
+    <t>ReinsNumber13_ctrl</t>
+  </si>
+  <si>
+    <t>A11125</t>
+  </si>
+  <si>
+    <t>A11126</t>
+  </si>
+  <si>
+    <t>ReinsNumber14_ctrl</t>
+  </si>
+  <si>
+    <t>A11127</t>
+  </si>
+  <si>
+    <t>A11128</t>
+  </si>
+  <si>
+    <t>ReinsNumber15_ctrl</t>
+  </si>
+  <si>
+    <t>A11130</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>using PortNumber/AccNumber/LocNumber filters, producing identical results.</t>
   </si>
 </sst>
 </file>
@@ -368,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,6 +761,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,9 +793,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -481,7 +833,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -587,7 +939,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -729,7 +1081,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -739,11 +1091,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2972,6 +3324,7 @@
   </sheetData>
   <autoFilter ref="A1:M64" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2979,7 +3332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C06D402-458E-4C8C-BE0A-253B6FFE4E88}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -3434,4 +3787,1545 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6CCBC3-4F4D-48BE-B1A5-32D1C3430D6A}">
+  <dimension ref="A1:T43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="S3" s="18"/>
+      <c r="T3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P4" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" t="s">
+        <v>110</v>
+      </c>
+      <c r="O5" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P5" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N6" t="s">
+        <v>113</v>
+      </c>
+      <c r="O6" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P6" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q6" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" t="s">
+        <v>115</v>
+      </c>
+      <c r="N7" t="s">
+        <v>116</v>
+      </c>
+      <c r="O7" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P7" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q7" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" t="s">
+        <v>119</v>
+      </c>
+      <c r="O8" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P8" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" t="s">
+        <v>120</v>
+      </c>
+      <c r="N9" t="s">
+        <v>121</v>
+      </c>
+      <c r="O9" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P9" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q9" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K10" t="s">
+        <v>125</v>
+      </c>
+      <c r="N10" t="s">
+        <v>126</v>
+      </c>
+      <c r="O10" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P10" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q10" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R10" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="K11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" t="s">
+        <v>130</v>
+      </c>
+      <c r="N11" t="s">
+        <v>131</v>
+      </c>
+      <c r="O11" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P11" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N12" t="s">
+        <v>134</v>
+      </c>
+      <c r="O12" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P12" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K13" t="s">
+        <v>129</v>
+      </c>
+      <c r="L13" t="s">
+        <v>140</v>
+      </c>
+      <c r="M13" t="s">
+        <v>141</v>
+      </c>
+      <c r="N13" t="s">
+        <v>142</v>
+      </c>
+      <c r="O13" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P13" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" t="s">
+        <v>144</v>
+      </c>
+      <c r="N14" t="s">
+        <v>145</v>
+      </c>
+      <c r="O14" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P14" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="J15" t="s">
+        <v>146</v>
+      </c>
+      <c r="N15" t="s">
+        <v>147</v>
+      </c>
+      <c r="O15" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P15" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>148</v>
+      </c>
+      <c r="K16" t="s">
+        <v>149</v>
+      </c>
+      <c r="N16" t="s">
+        <v>150</v>
+      </c>
+      <c r="O16" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P16" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L17" t="s">
+        <v>151</v>
+      </c>
+      <c r="N17" t="s">
+        <v>152</v>
+      </c>
+      <c r="O17" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P17" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" t="s">
+        <v>154</v>
+      </c>
+      <c r="N18" t="s">
+        <v>155</v>
+      </c>
+      <c r="O18" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P18" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q18" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>153</v>
+      </c>
+      <c r="M19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N19" t="s">
+        <v>157</v>
+      </c>
+      <c r="O19" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P19" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q19" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" t="s">
+        <v>159</v>
+      </c>
+      <c r="L20" t="s">
+        <v>160</v>
+      </c>
+      <c r="N20" t="s">
+        <v>161</v>
+      </c>
+      <c r="O20" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P20" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>158</v>
+      </c>
+      <c r="L21" t="s">
+        <v>160</v>
+      </c>
+      <c r="M21" t="s">
+        <v>162</v>
+      </c>
+      <c r="N21" t="s">
+        <v>163</v>
+      </c>
+      <c r="O21" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P21" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q21" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>165</v>
+      </c>
+      <c r="H22">
+        <v>19</v>
+      </c>
+      <c r="N22" t="s">
+        <v>166</v>
+      </c>
+      <c r="O22" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P22" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q22" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>164</v>
+      </c>
+      <c r="L23" t="s">
+        <v>167</v>
+      </c>
+      <c r="N23" t="s">
+        <v>168</v>
+      </c>
+      <c r="O23" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P23" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q23" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24">
+        <v>101</v>
+      </c>
+      <c r="F24" t="s">
+        <v>170</v>
+      </c>
+      <c r="N24" t="s">
+        <v>107</v>
+      </c>
+      <c r="O24" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P24" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25">
+        <v>101</v>
+      </c>
+      <c r="F25" t="s">
+        <v>172</v>
+      </c>
+      <c r="N25" t="s">
+        <v>110</v>
+      </c>
+      <c r="O25" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P25" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q25" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26">
+        <v>101</v>
+      </c>
+      <c r="F26" t="s">
+        <v>174</v>
+      </c>
+      <c r="N26" t="s">
+        <v>113</v>
+      </c>
+      <c r="O26" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P26" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q26" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27">
+        <v>101</v>
+      </c>
+      <c r="F27" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="N27" t="s">
+        <v>116</v>
+      </c>
+      <c r="O27" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P27" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q27" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28">
+        <v>101</v>
+      </c>
+      <c r="F28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="N28" t="s">
+        <v>119</v>
+      </c>
+      <c r="O28" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P28" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q28" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>179</v>
+      </c>
+      <c r="E29">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>180</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="N29" t="s">
+        <v>121</v>
+      </c>
+      <c r="O29" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P29" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q29" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
+        <v>182</v>
+      </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="N30" t="s">
+        <v>126</v>
+      </c>
+      <c r="O30" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P30" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q30" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31">
+        <v>102</v>
+      </c>
+      <c r="F31" t="s">
+        <v>184</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="N31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O31" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P31" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q31" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>186</v>
+      </c>
+      <c r="H32">
+        <v>9</v>
+      </c>
+      <c r="N32" t="s">
+        <v>134</v>
+      </c>
+      <c r="O32" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P32" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q32" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>110</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <v>0.5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>187</v>
+      </c>
+      <c r="E33">
+        <v>102</v>
+      </c>
+      <c r="F33" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="N33" t="s">
+        <v>142</v>
+      </c>
+      <c r="O33" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P33" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q33" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>111</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34">
+        <v>103</v>
+      </c>
+      <c r="F34" t="s">
+        <v>190</v>
+      </c>
+      <c r="N34" t="s">
+        <v>145</v>
+      </c>
+      <c r="O34" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P34" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q34" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35">
+        <v>0.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35">
+        <v>103</v>
+      </c>
+      <c r="F35" t="s">
+        <v>191</v>
+      </c>
+      <c r="N35" t="s">
+        <v>147</v>
+      </c>
+      <c r="O35" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P35" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q35" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36">
+        <v>103</v>
+      </c>
+      <c r="F36" t="s">
+        <v>193</v>
+      </c>
+      <c r="N36" t="s">
+        <v>150</v>
+      </c>
+      <c r="O36" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P36" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q36" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>0.5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37">
+        <v>103</v>
+      </c>
+      <c r="F37" t="s">
+        <v>194</v>
+      </c>
+      <c r="H37">
+        <v>14</v>
+      </c>
+      <c r="N37" t="s">
+        <v>152</v>
+      </c>
+      <c r="O37" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P37" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q37" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>0.5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38">
+        <v>103</v>
+      </c>
+      <c r="F38" t="s">
+        <v>196</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="N38" t="s">
+        <v>155</v>
+      </c>
+      <c r="O38" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P38" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q38" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>0.5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39">
+        <v>104</v>
+      </c>
+      <c r="F39" t="s">
+        <v>197</v>
+      </c>
+      <c r="H39">
+        <v>16</v>
+      </c>
+      <c r="N39" t="s">
+        <v>157</v>
+      </c>
+      <c r="O39" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P39" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q39" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>114</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>0.5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>198</v>
+      </c>
+      <c r="E40">
+        <v>104</v>
+      </c>
+      <c r="F40" t="s">
+        <v>199</v>
+      </c>
+      <c r="H40">
+        <v>17</v>
+      </c>
+      <c r="N40" t="s">
+        <v>161</v>
+      </c>
+      <c r="O40" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P40" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q40" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>114</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>0.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41">
+        <v>104</v>
+      </c>
+      <c r="F41" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41">
+        <v>18</v>
+      </c>
+      <c r="N41" t="s">
+        <v>163</v>
+      </c>
+      <c r="O41" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P41" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q41" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42">
+        <v>0.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42">
+        <v>104</v>
+      </c>
+      <c r="F42" t="s">
+        <v>165</v>
+      </c>
+      <c r="H42">
+        <v>19</v>
+      </c>
+      <c r="N42" t="s">
+        <v>166</v>
+      </c>
+      <c r="O42" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P42" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q42" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>115</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <v>0.5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>201</v>
+      </c>
+      <c r="E43">
+        <v>104</v>
+      </c>
+      <c r="F43" t="s">
+        <v>202</v>
+      </c>
+      <c r="H43">
+        <v>20</v>
+      </c>
+      <c r="N43" t="s">
+        <v>168</v>
+      </c>
+      <c r="O43" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P43" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q43" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
support ri_scope filter (#1505)
* support ri_scope filter

* added ri scope test folder

* pep8

* added more ri scope filter tests with expected folder and updated doc

* remove obsolete ri unit tests

* fixup

---------

Co-authored-by: Joh Carter <johanna.carter@oasislmf.org>
</commit_message>
<xml_diff>
--- a/validation/reinsurance_test_case_list.xlsx
+++ b/validation/reinsurance_test_case_list.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_branch\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\joh\dev\OasisLMF_ri_scope\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FC181F-E676-4647-81EF-2D023E588705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25008196-2B24-4669-A4C5-5D59061144B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
   </bookViews>
   <sheets>
     <sheet name="reinsurance1" sheetId="1" r:id="rId1"/>
     <sheet name="reinsurance2" sheetId="2" r:id="rId2"/>
+    <sheet name="reinsurance3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">reinsurance1!$A$1:$M$64</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="205">
   <si>
     <t>FolderName</t>
   </si>
@@ -304,6 +305,354 @@
   </si>
   <si>
     <t>single contract tests</t>
+  </si>
+  <si>
+    <t>reinsurance 3 ri scope filter test list</t>
+  </si>
+  <si>
+    <t>PlacedPercent</t>
+  </si>
+  <si>
+    <t>ReinsName</t>
+  </si>
+  <si>
+    <t>PortNumber</t>
+  </si>
+  <si>
+    <t>AccNumber</t>
+  </si>
+  <si>
+    <t>LocGroup</t>
+  </si>
+  <si>
+    <t>LocNumber</t>
+  </si>
+  <si>
+    <t>CedantName</t>
+  </si>
+  <si>
+    <t>ProducerName</t>
+  </si>
+  <si>
+    <t>LOB</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>ReinsTag</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Cedant1</t>
+  </si>
+  <si>
+    <t>50% of Loc1 ceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These filter tests are designed to </t>
+  </si>
+  <si>
+    <t>Producer2</t>
+  </si>
+  <si>
+    <t>50% of Loc2 ceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">result in each unique location being ceded 50% in total, </t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>50% of Loc3 ceded</t>
+  </si>
+  <si>
+    <t>across all reinsurance contracts</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>50% of Loc4 ceded</t>
+  </si>
+  <si>
+    <t>resulting in all net losses by location being 50% of the gross loss.</t>
+  </si>
+  <si>
+    <t>ReinsTag5</t>
+  </si>
+  <si>
+    <t>50% of Loc5 ceded</t>
+  </si>
+  <si>
+    <t>LocGroup6</t>
+  </si>
+  <si>
+    <t>50% of Loc6 ceded</t>
+  </si>
+  <si>
+    <t>ReinsNumber 1-15 are the tests for the filter fields;</t>
+  </si>
+  <si>
+    <t>Cedant7 and COM</t>
+  </si>
+  <si>
+    <t>Cedant7</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>50% of Loc7 ceded</t>
+  </si>
+  <si>
+    <t>CedantName, ProducerName, LOB, LocGroup, ReinsTag</t>
+  </si>
+  <si>
+    <t>IND and IE</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>50% of Loc8 ceded</t>
+  </si>
+  <si>
+    <t>COM and ReinsTag9</t>
+  </si>
+  <si>
+    <t>ReinsTag9</t>
+  </si>
+  <si>
+    <t>50% of Loc9 ceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReinsNumber 101-115 are the equivalent tests to ReinsNumber 1-15 </t>
+  </si>
+  <si>
+    <t>All Loc 10 filters</t>
+  </si>
+  <si>
+    <t>LocGroup10</t>
+  </si>
+  <si>
+    <t>Cedant10</t>
+  </si>
+  <si>
+    <t>Producer10</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>ReinsTag10</t>
+  </si>
+  <si>
+    <t>50% of Loc10 ceded</t>
+  </si>
+  <si>
+    <t>Cedant11 or Producer12</t>
+  </si>
+  <si>
+    <t>Cedant11</t>
+  </si>
+  <si>
+    <t>50% of Loc11 ceded</t>
+  </si>
+  <si>
+    <t>Producer12</t>
+  </si>
+  <si>
+    <t>50% of Loc12 ceded</t>
+  </si>
+  <si>
+    <t>AGR or AT</t>
+  </si>
+  <si>
+    <t>AGR</t>
+  </si>
+  <si>
+    <t>50% of Loc13 ceded</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>50% of Loc14 ceded</t>
+  </si>
+  <si>
+    <t>LocGroup15 or ReinsTag16</t>
+  </si>
+  <si>
+    <t>LocGroup15</t>
+  </si>
+  <si>
+    <t>50% of Loc15 ceded</t>
+  </si>
+  <si>
+    <t>ReinsTag16</t>
+  </si>
+  <si>
+    <t>50% of Loc16 ceded</t>
+  </si>
+  <si>
+    <t>Cedant17 and IT or IT and ReinsTag18</t>
+  </si>
+  <si>
+    <t>Cedant17</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>50% of Loc17 ceded</t>
+  </si>
+  <si>
+    <t>ReinsTag18</t>
+  </si>
+  <si>
+    <t>50% of Loc18 ceded</t>
+  </si>
+  <si>
+    <t>Port4 Loc19 or CH</t>
+  </si>
+  <si>
+    <t>A11129</t>
+  </si>
+  <si>
+    <t>50% of Loc19 ceded</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>50% of Loc20 ceded</t>
+  </si>
+  <si>
+    <t>ReinsNumber1_ctrl</t>
+  </si>
+  <si>
+    <t>A11111</t>
+  </si>
+  <si>
+    <t>ReinsNumber2_ctrl</t>
+  </si>
+  <si>
+    <t>A11112</t>
+  </si>
+  <si>
+    <t>ReinsNumber3_ctrl</t>
+  </si>
+  <si>
+    <t>A11113</t>
+  </si>
+  <si>
+    <t>ReinsNumber4_ctrl</t>
+  </si>
+  <si>
+    <t>A11114</t>
+  </si>
+  <si>
+    <t>ReinsNumber5_ctrl</t>
+  </si>
+  <si>
+    <t>A11115</t>
+  </si>
+  <si>
+    <t>ReinsNumber6_ctrl</t>
+  </si>
+  <si>
+    <t>A11116</t>
+  </si>
+  <si>
+    <t>ReinsNumber7_ctrl</t>
+  </si>
+  <si>
+    <t>A11117</t>
+  </si>
+  <si>
+    <t>ReinsNumber8_ctrl</t>
+  </si>
+  <si>
+    <t>A11118</t>
+  </si>
+  <si>
+    <t>ReinsNumber9_ctrl</t>
+  </si>
+  <si>
+    <t>A11119</t>
+  </si>
+  <si>
+    <t>ReinsNumber10_ctrl</t>
+  </si>
+  <si>
+    <t>A11120</t>
+  </si>
+  <si>
+    <t>ReinsNumber11_ctrl</t>
+  </si>
+  <si>
+    <t>A11121</t>
+  </si>
+  <si>
+    <t>A11122</t>
+  </si>
+  <si>
+    <t>ReinsNumber12_ctrl</t>
+  </si>
+  <si>
+    <t>A11123</t>
+  </si>
+  <si>
+    <t>A11124</t>
+  </si>
+  <si>
+    <t>ReinsNumber13_ctrl</t>
+  </si>
+  <si>
+    <t>A11125</t>
+  </si>
+  <si>
+    <t>A11126</t>
+  </si>
+  <si>
+    <t>ReinsNumber14_ctrl</t>
+  </si>
+  <si>
+    <t>A11127</t>
+  </si>
+  <si>
+    <t>A11128</t>
+  </si>
+  <si>
+    <t>ReinsNumber15_ctrl</t>
+  </si>
+  <si>
+    <t>A11130</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>using PortNumber/AccNumber/LocNumber filters, producing identical results.</t>
   </si>
 </sst>
 </file>
@@ -368,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,6 +761,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,9 +793,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -481,7 +833,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -587,7 +939,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -729,7 +1081,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -739,11 +1091,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2972,6 +3324,7 @@
   </sheetData>
   <autoFilter ref="A1:M64" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2979,7 +3332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C06D402-458E-4C8C-BE0A-253B6FFE4E88}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -3434,4 +3787,1545 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6CCBC3-4F4D-48BE-B1A5-32D1C3430D6A}">
+  <dimension ref="A1:T43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="S3" s="18"/>
+      <c r="T3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P4" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" t="s">
+        <v>110</v>
+      </c>
+      <c r="O5" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P5" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N6" t="s">
+        <v>113</v>
+      </c>
+      <c r="O6" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P6" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q6" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" t="s">
+        <v>115</v>
+      </c>
+      <c r="N7" t="s">
+        <v>116</v>
+      </c>
+      <c r="O7" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P7" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q7" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" t="s">
+        <v>119</v>
+      </c>
+      <c r="O8" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P8" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" t="s">
+        <v>120</v>
+      </c>
+      <c r="N9" t="s">
+        <v>121</v>
+      </c>
+      <c r="O9" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P9" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q9" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K10" t="s">
+        <v>125</v>
+      </c>
+      <c r="N10" t="s">
+        <v>126</v>
+      </c>
+      <c r="O10" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P10" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q10" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R10" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="K11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" t="s">
+        <v>130</v>
+      </c>
+      <c r="N11" t="s">
+        <v>131</v>
+      </c>
+      <c r="O11" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P11" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N12" t="s">
+        <v>134</v>
+      </c>
+      <c r="O12" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P12" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K13" t="s">
+        <v>129</v>
+      </c>
+      <c r="L13" t="s">
+        <v>140</v>
+      </c>
+      <c r="M13" t="s">
+        <v>141</v>
+      </c>
+      <c r="N13" t="s">
+        <v>142</v>
+      </c>
+      <c r="O13" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P13" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" t="s">
+        <v>144</v>
+      </c>
+      <c r="N14" t="s">
+        <v>145</v>
+      </c>
+      <c r="O14" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P14" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="J15" t="s">
+        <v>146</v>
+      </c>
+      <c r="N15" t="s">
+        <v>147</v>
+      </c>
+      <c r="O15" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P15" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>148</v>
+      </c>
+      <c r="K16" t="s">
+        <v>149</v>
+      </c>
+      <c r="N16" t="s">
+        <v>150</v>
+      </c>
+      <c r="O16" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P16" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L17" t="s">
+        <v>151</v>
+      </c>
+      <c r="N17" t="s">
+        <v>152</v>
+      </c>
+      <c r="O17" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P17" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" t="s">
+        <v>154</v>
+      </c>
+      <c r="N18" t="s">
+        <v>155</v>
+      </c>
+      <c r="O18" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P18" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q18" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>153</v>
+      </c>
+      <c r="M19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N19" t="s">
+        <v>157</v>
+      </c>
+      <c r="O19" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P19" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q19" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" t="s">
+        <v>159</v>
+      </c>
+      <c r="L20" t="s">
+        <v>160</v>
+      </c>
+      <c r="N20" t="s">
+        <v>161</v>
+      </c>
+      <c r="O20" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P20" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>158</v>
+      </c>
+      <c r="L21" t="s">
+        <v>160</v>
+      </c>
+      <c r="M21" t="s">
+        <v>162</v>
+      </c>
+      <c r="N21" t="s">
+        <v>163</v>
+      </c>
+      <c r="O21" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P21" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q21" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>165</v>
+      </c>
+      <c r="H22">
+        <v>19</v>
+      </c>
+      <c r="N22" t="s">
+        <v>166</v>
+      </c>
+      <c r="O22" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P22" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q22" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>164</v>
+      </c>
+      <c r="L23" t="s">
+        <v>167</v>
+      </c>
+      <c r="N23" t="s">
+        <v>168</v>
+      </c>
+      <c r="O23" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P23" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q23" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24">
+        <v>101</v>
+      </c>
+      <c r="F24" t="s">
+        <v>170</v>
+      </c>
+      <c r="N24" t="s">
+        <v>107</v>
+      </c>
+      <c r="O24" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P24" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25">
+        <v>101</v>
+      </c>
+      <c r="F25" t="s">
+        <v>172</v>
+      </c>
+      <c r="N25" t="s">
+        <v>110</v>
+      </c>
+      <c r="O25" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P25" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q25" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26">
+        <v>101</v>
+      </c>
+      <c r="F26" t="s">
+        <v>174</v>
+      </c>
+      <c r="N26" t="s">
+        <v>113</v>
+      </c>
+      <c r="O26" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P26" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q26" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27">
+        <v>101</v>
+      </c>
+      <c r="F27" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="N27" t="s">
+        <v>116</v>
+      </c>
+      <c r="O27" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P27" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q27" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28">
+        <v>101</v>
+      </c>
+      <c r="F28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="N28" t="s">
+        <v>119</v>
+      </c>
+      <c r="O28" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P28" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q28" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>179</v>
+      </c>
+      <c r="E29">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>180</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="N29" t="s">
+        <v>121</v>
+      </c>
+      <c r="O29" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P29" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q29" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
+        <v>182</v>
+      </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="N30" t="s">
+        <v>126</v>
+      </c>
+      <c r="O30" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P30" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q30" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31">
+        <v>102</v>
+      </c>
+      <c r="F31" t="s">
+        <v>184</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="N31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O31" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P31" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q31" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>186</v>
+      </c>
+      <c r="H32">
+        <v>9</v>
+      </c>
+      <c r="N32" t="s">
+        <v>134</v>
+      </c>
+      <c r="O32" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P32" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q32" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>110</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <v>0.5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>187</v>
+      </c>
+      <c r="E33">
+        <v>102</v>
+      </c>
+      <c r="F33" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="N33" t="s">
+        <v>142</v>
+      </c>
+      <c r="O33" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P33" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q33" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>111</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34">
+        <v>103</v>
+      </c>
+      <c r="F34" t="s">
+        <v>190</v>
+      </c>
+      <c r="N34" t="s">
+        <v>145</v>
+      </c>
+      <c r="O34" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P34" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q34" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35">
+        <v>0.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35">
+        <v>103</v>
+      </c>
+      <c r="F35" t="s">
+        <v>191</v>
+      </c>
+      <c r="N35" t="s">
+        <v>147</v>
+      </c>
+      <c r="O35" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P35" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q35" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36">
+        <v>103</v>
+      </c>
+      <c r="F36" t="s">
+        <v>193</v>
+      </c>
+      <c r="N36" t="s">
+        <v>150</v>
+      </c>
+      <c r="O36" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P36" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q36" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>0.5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37">
+        <v>103</v>
+      </c>
+      <c r="F37" t="s">
+        <v>194</v>
+      </c>
+      <c r="H37">
+        <v>14</v>
+      </c>
+      <c r="N37" t="s">
+        <v>152</v>
+      </c>
+      <c r="O37" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P37" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q37" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>0.5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38">
+        <v>103</v>
+      </c>
+      <c r="F38" t="s">
+        <v>196</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="N38" t="s">
+        <v>155</v>
+      </c>
+      <c r="O38" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P38" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q38" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>0.5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39">
+        <v>104</v>
+      </c>
+      <c r="F39" t="s">
+        <v>197</v>
+      </c>
+      <c r="H39">
+        <v>16</v>
+      </c>
+      <c r="N39" t="s">
+        <v>157</v>
+      </c>
+      <c r="O39" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P39" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q39" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>114</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>0.5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>198</v>
+      </c>
+      <c r="E40">
+        <v>104</v>
+      </c>
+      <c r="F40" t="s">
+        <v>199</v>
+      </c>
+      <c r="H40">
+        <v>17</v>
+      </c>
+      <c r="N40" t="s">
+        <v>161</v>
+      </c>
+      <c r="O40" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P40" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q40" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>114</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>0.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41">
+        <v>104</v>
+      </c>
+      <c r="F41" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41">
+        <v>18</v>
+      </c>
+      <c r="N41" t="s">
+        <v>163</v>
+      </c>
+      <c r="O41" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P41" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q41" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42">
+        <v>0.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42">
+        <v>104</v>
+      </c>
+      <c r="F42" t="s">
+        <v>165</v>
+      </c>
+      <c r="H42">
+        <v>19</v>
+      </c>
+      <c r="N42" t="s">
+        <v>166</v>
+      </c>
+      <c r="O42" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P42" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q42" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>115</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <v>0.5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>201</v>
+      </c>
+      <c r="E43">
+        <v>104</v>
+      </c>
+      <c r="F43" t="s">
+        <v>202</v>
+      </c>
+      <c r="H43">
+        <v>20</v>
+      </c>
+      <c r="N43" t="s">
+        <v>168</v>
+      </c>
+      <c r="O43" s="17">
+        <v>150000</v>
+      </c>
+      <c r="P43" s="17">
+        <v>15000</v>
+      </c>
+      <c r="Q43" s="17">
+        <v>7500</v>
+      </c>
+      <c r="R43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>